<commit_message>
Total Number of days added
</commit_message>
<xml_diff>
--- a/excel gpio.xlsx
+++ b/excel gpio.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohith\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chetan\gpio_vip\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>S.NO</t>
   </si>
   <si>
-    <t xml:space="preserve">Expected Days required </t>
-  </si>
-  <si>
     <t>Stages</t>
   </si>
   <si>
@@ -47,23 +44,50 @@
     <t>Test Cases</t>
   </si>
   <si>
-    <t>overall Evaluation</t>
-  </si>
-  <si>
     <t>GPIO_VIP Road Maps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected Days Required </t>
+  </si>
+  <si>
+    <t>Overall Evaluation</t>
+  </si>
+  <si>
+    <t>Total Days</t>
+  </si>
+  <si>
+    <t>20 days</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,12 +119,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -124,7 +152,7 @@
   <tableColumns count="3">
     <tableColumn id="1" name="S.NO"/>
     <tableColumn id="2" name="Stages"/>
-    <tableColumn id="3" name="Expected Days required "/>
+    <tableColumn id="3" name="Expected Days Required "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -396,19 +424,19 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="A8" sqref="A8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -418,10 +446,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -429,7 +457,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -440,7 +468,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -451,7 +479,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -462,7 +490,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -473,10 +501,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="7:7" x14ac:dyDescent="0.25">
@@ -487,8 +524,9 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>